<commit_message>
actualizo tp_roberto.ipynb con 10 columnas nuevas extraidas del campo description
</commit_message>
<xml_diff>
--- a/Datos generales del file.xlsx
+++ b/Datos generales del file.xlsx
@@ -1,42 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VivoBook\Documents\Roberto\_Data_Science_curso\221018 Tp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AB5FE060-CBC0-A44F-B1FC-4EA729310276}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11916" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11916"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="104">
   <si>
     <t>data = pd.read_csv('C:/Users/VivoBook/Documents/Roberto/_Data_Science_curso/221018 Tp/properatti.csv', index_col=0)</t>
   </si>
@@ -1095,12 +1083,81 @@
   </si>
   <si>
     <t>114389 diferentes</t>
+  </si>
+  <si>
+    <t>agregados</t>
+  </si>
+  <si>
+    <t>ambientes</t>
+  </si>
+  <si>
+    <t>10292 no nulos - donde rooms es nulo</t>
+  </si>
+  <si>
+    <t>baños</t>
+  </si>
+  <si>
+    <t>dormitorios</t>
+  </si>
+  <si>
+    <t>balcon</t>
+  </si>
+  <si>
+    <t>bool</t>
+  </si>
+  <si>
+    <t>str - pero es un número</t>
+  </si>
+  <si>
+    <t>cochera</t>
+  </si>
+  <si>
+    <t>41977 True</t>
+  </si>
+  <si>
+    <t>37149 True</t>
+  </si>
+  <si>
+    <t>34366 no nulos</t>
+  </si>
+  <si>
+    <t>9965 no nulos</t>
+  </si>
+  <si>
+    <t>jardin</t>
+  </si>
+  <si>
+    <t>15334 True</t>
+  </si>
+  <si>
+    <t>lavadero</t>
+  </si>
+  <si>
+    <t>32707 True</t>
+  </si>
+  <si>
+    <t>parrilla</t>
+  </si>
+  <si>
+    <t>29778 True</t>
+  </si>
+  <si>
+    <t>patio</t>
+  </si>
+  <si>
+    <t>17269 True</t>
+  </si>
+  <si>
+    <t>pileta</t>
+  </si>
+  <si>
+    <t>28821 True</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1430,26 +1487,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:O29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:O40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.76171875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="4.83984375" customWidth="1"/>
-    <col min="7" max="7" width="4.83984375" customWidth="1"/>
-    <col min="11" max="11" width="4.83984375" customWidth="1"/>
+    <col min="3" max="3" width="4.77734375" customWidth="1"/>
+    <col min="7" max="7" width="4.77734375" customWidth="1"/>
+    <col min="11" max="11" width="4.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
         <v>27</v>
       </c>
@@ -1464,7 +1521,7 @@
       </c>
       <c r="O3" s="2"/>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>28</v>
       </c>
@@ -1481,7 +1538,7 @@
         <v>121220</v>
       </c>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
       <c r="D5" t="s">
         <v>5</v>
       </c>
@@ -1492,7 +1549,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
       <c r="D6" t="s">
         <v>33</v>
       </c>
@@ -1503,7 +1560,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
       <c r="D7" t="s">
         <v>6</v>
       </c>
@@ -1514,7 +1571,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
       <c r="D8" t="s">
         <v>7</v>
       </c>
@@ -1528,7 +1585,7 @@
         <v>121220</v>
       </c>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.3">
       <c r="D9" t="s">
         <v>8</v>
       </c>
@@ -1539,7 +1596,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.3">
       <c r="D10" t="s">
         <v>9</v>
       </c>
@@ -1550,7 +1607,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.3">
       <c r="D11" t="s">
         <v>11</v>
       </c>
@@ -1561,7 +1618,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
       <c r="D12" t="s">
         <v>10</v>
       </c>
@@ -1572,7 +1629,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
       <c r="D13" t="s">
         <v>12</v>
       </c>
@@ -1583,7 +1640,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
       <c r="D14" t="s">
         <v>13</v>
       </c>
@@ -1594,7 +1651,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.3">
       <c r="D15" t="s">
         <v>14</v>
       </c>
@@ -1605,7 +1662,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:15" x14ac:dyDescent="0.3">
       <c r="D16" t="s">
         <v>2</v>
       </c>
@@ -1616,7 +1673,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
       <c r="D17" t="s">
         <v>15</v>
       </c>
@@ -1627,7 +1684,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
       <c r="D18" t="s">
         <v>16</v>
       </c>
@@ -1638,7 +1695,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="19" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
       <c r="D19" t="s">
         <v>17</v>
       </c>
@@ -1649,7 +1706,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
       <c r="D20" t="s">
         <v>18</v>
       </c>
@@ -1660,7 +1717,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="21" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
       <c r="D21" t="s">
         <v>19</v>
       </c>
@@ -1671,7 +1728,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.3">
       <c r="D22" t="s">
         <v>20</v>
       </c>
@@ -1682,7 +1739,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="23" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.3">
       <c r="D23" t="s">
         <v>21</v>
       </c>
@@ -1693,7 +1750,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="24" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.3">
       <c r="D24" t="s">
         <v>22</v>
       </c>
@@ -1704,7 +1761,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="25" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:12" x14ac:dyDescent="0.3">
       <c r="D25" t="s">
         <v>23</v>
       </c>
@@ -1715,7 +1772,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="26" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:12" x14ac:dyDescent="0.3">
       <c r="D26" t="s">
         <v>24</v>
       </c>
@@ -1726,7 +1783,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="27" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:12" x14ac:dyDescent="0.3">
       <c r="D27" t="s">
         <v>25</v>
       </c>
@@ -1737,7 +1794,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="28" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:12" x14ac:dyDescent="0.3">
       <c r="D28" t="s">
         <v>26</v>
       </c>
@@ -1748,9 +1805,122 @@
         <v>80</v>
       </c>
     </row>
-    <row r="29" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:12" x14ac:dyDescent="0.3">
       <c r="D29" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>81</v>
+      </c>
+      <c r="D31" t="s">
+        <v>82</v>
+      </c>
+      <c r="F31" t="s">
+        <v>88</v>
+      </c>
+      <c r="I31" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="D32" t="s">
+        <v>84</v>
+      </c>
+      <c r="F32" t="s">
+        <v>88</v>
+      </c>
+      <c r="I32" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="33" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D33" t="s">
+        <v>85</v>
+      </c>
+      <c r="F33" t="s">
+        <v>88</v>
+      </c>
+      <c r="I33" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="34" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D34" t="s">
+        <v>86</v>
+      </c>
+      <c r="F34" t="s">
+        <v>87</v>
+      </c>
+      <c r="I34" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="35" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D35" t="s">
+        <v>89</v>
+      </c>
+      <c r="F35" t="s">
+        <v>87</v>
+      </c>
+      <c r="I35" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="36" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D36" t="s">
+        <v>94</v>
+      </c>
+      <c r="F36" t="s">
+        <v>87</v>
+      </c>
+      <c r="I36" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="37" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D37" t="s">
+        <v>96</v>
+      </c>
+      <c r="F37" t="s">
+        <v>87</v>
+      </c>
+      <c r="I37" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="38" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D38" t="s">
+        <v>98</v>
+      </c>
+      <c r="F38" t="s">
+        <v>87</v>
+      </c>
+      <c r="I38" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="39" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D39" t="s">
+        <v>100</v>
+      </c>
+      <c r="F39" t="s">
+        <v>87</v>
+      </c>
+      <c r="I39" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="40" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D40" t="s">
+        <v>102</v>
+      </c>
+      <c r="F40" t="s">
+        <v>87</v>
+      </c>
+      <c r="I40" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
agrego columnas excelente y vista
</commit_message>
<xml_diff>
--- a/Datos generales del file.xlsx
+++ b/Datos generales del file.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="108">
   <si>
     <t>data = pd.read_csv('C:/Users/VivoBook/Documents/Roberto/_Data_Science_curso/221018 Tp/properatti.csv', index_col=0)</t>
   </si>
@@ -1152,6 +1152,18 @@
   </si>
   <si>
     <t>28821 True</t>
+  </si>
+  <si>
+    <t>excelente</t>
+  </si>
+  <si>
+    <t>vista</t>
+  </si>
+  <si>
+    <t>33376 True</t>
+  </si>
+  <si>
+    <t>15444 True</t>
   </si>
 </sst>
 </file>
@@ -1488,10 +1500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:O40"/>
+  <dimension ref="B2:O42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1923,6 +1935,28 @@
         <v>103</v>
       </c>
     </row>
+    <row r="41" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D41" t="s">
+        <v>104</v>
+      </c>
+      <c r="F41" t="s">
+        <v>87</v>
+      </c>
+      <c r="I41" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="42" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D42" t="s">
+        <v>105</v>
+      </c>
+      <c r="F42" t="s">
+        <v>87</v>
+      </c>
+      <c r="I42" t="s">
+        <v>106</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
agregué columna nueva usdm2
</commit_message>
<xml_diff>
--- a/Datos generales del file.xlsx
+++ b/Datos generales del file.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="116">
   <si>
     <t>data = pd.read_csv('C:/Users/VivoBook/Documents/Roberto/_Data_Science_curso/221018 Tp/properatti.csv', index_col=0)</t>
   </si>
@@ -1164,6 +1164,30 @@
   </si>
   <si>
     <t>15444 True</t>
+  </si>
+  <si>
+    <t>usd_per_m2_2</t>
+  </si>
+  <si>
+    <t>float64</t>
+  </si>
+  <si>
+    <t>17817 no nulos</t>
+  </si>
+  <si>
+    <t>provincia_ciudad</t>
+  </si>
+  <si>
+    <t>str</t>
+  </si>
+  <si>
+    <t>provincia si es el interior - capital - bsas zona sur o zona norte</t>
+  </si>
+  <si>
+    <t>ciudad_barrio</t>
+  </si>
+  <si>
+    <t>ciudad si es el interior - barrio si es capital</t>
   </si>
 </sst>
 </file>
@@ -1500,10 +1524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:O42"/>
+  <dimension ref="B2:O45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I46" sqref="I46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1957,6 +1981,39 @@
         <v>106</v>
       </c>
     </row>
+    <row r="43" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D43" t="s">
+        <v>108</v>
+      </c>
+      <c r="F43" t="s">
+        <v>109</v>
+      </c>
+      <c r="I43" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="44" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D44" t="s">
+        <v>111</v>
+      </c>
+      <c r="F44" t="s">
+        <v>112</v>
+      </c>
+      <c r="I44" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="45" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D45" t="s">
+        <v>114</v>
+      </c>
+      <c r="F45" t="s">
+        <v>112</v>
+      </c>
+      <c r="I45" t="s">
+        <v>115</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>